<commit_message>
throwback16 > slider > full with slider
</commit_message>
<xml_diff>
--- a/docs/Etapes Projet Prestashop.xlsx
+++ b/docs/Etapes Projet Prestashop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Steps" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="239">
   <si>
     <t xml:space="preserve">Périmètre Fonctionelle </t>
   </si>
@@ -982,6 +982,33 @@
   </si>
   <si>
     <t>Centrer Menu Horizontale</t>
+  </si>
+  <si>
+    <t>SLIDER SUR TOUTE LA LARGEUR SUR VOTRE PAGE D’ACCUEIL</t>
+  </si>
+  <si>
+    <t>http://www.majory-cubizolles.fr/blog/slider-sur-toute-la-largeur-de-la-home/</t>
+  </si>
+  <si>
+    <t>Centrer les sous menu</t>
+  </si>
+  <si>
+    <t>images PNG</t>
+  </si>
+  <si>
+    <t>préférences &gt; images &gt; charger JPEG quand c'est leformat d'origine</t>
+  </si>
+  <si>
+    <t>Slider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centrer le slider </t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Changer la taille des images dans le tpl du module</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1340,7 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1444,6 +1471,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Calcul" xfId="2" builtinId="22"/>
@@ -2216,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2543,6 +2571,17 @@
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="20" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C59" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2571,10 +2610,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2727,7 +2766,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" s="43"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>129</v>
       </c>
@@ -2735,10 +2774,10 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C18" s="43"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
         <v>166</v>
       </c>
@@ -2746,7 +2785,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
         <v>131</v>
       </c>
@@ -2754,19 +2793,19 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C21" s="43"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C22" s="43"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C23" s="43"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C24" s="43"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
         <v>160</v>
       </c>
@@ -2774,7 +2813,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
         <v>157</v>
       </c>
@@ -2782,7 +2821,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -2792,23 +2831,57 @@
       <c r="C28" s="22" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>228</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1"/>
+    <hyperlink ref="B31" r:id="rId2"/>
+    <hyperlink ref="B29" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2944,7 +3017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
blog > add dumpfile
</commit_message>
<xml_diff>
--- a/docs/Etapes Projet Prestashop.xlsx
+++ b/docs/Etapes Projet Prestashop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Steps" sheetId="4" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Manip - heme" sheetId="6" r:id="rId4"/>
     <sheet name="Feuil1" sheetId="1" r:id="rId5"/>
     <sheet name="Default Theme Layout" sheetId="3" r:id="rId6"/>
+    <sheet name="WP Install Steps" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="256">
   <si>
     <t xml:space="preserve">Périmètre Fonctionelle </t>
   </si>
@@ -1010,12 +1011,90 @@
   <si>
     <t>Changer la taille des images dans le tpl du module</t>
   </si>
+  <si>
+    <t>installer wordpress 4.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">créer base de données pour le blog </t>
+  </si>
+  <si>
+    <t>CREATE DATABASE IF NOT EXISTS throwbackwordpress
+GRANT ALL PRIVILEGES ON throwbackwordpress.* TO 'usertbwp'@'localhost' IDENTIFIED BY 'pwdtbwp';</t>
+  </si>
+  <si>
+    <t>créant un répertoire blog dans le dossier prestashop</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF282828"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF282828"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>installer wordpress dans le répertoire</t>
+    </r>
+  </si>
+  <si>
+    <t>https://codex.wordpress.org/fr:Installer_WordPress</t>
+  </si>
+  <si>
+    <t>https://fr.wordpress.org/themes/</t>
+  </si>
+  <si>
+    <t>Installer plugins</t>
+  </si>
+  <si>
+    <t>Configuration de Base</t>
+  </si>
+  <si>
+    <t>Import des articles de l'ancien blog</t>
+  </si>
+  <si>
+    <t>Dupliquer thème</t>
+  </si>
+  <si>
+    <t>intégration Prestashop &amp; WordPress</t>
+  </si>
+  <si>
+    <t>Choisir/activer thème de base : twentyseventeen</t>
+  </si>
+  <si>
+    <t>Intégrer le Header &amp; footer de PS dans le thème WP</t>
+  </si>
+  <si>
+    <t>https://www.webbax.ch/2016/02/24/ajouter-wordpress-a-prestashop-1-6/</t>
+  </si>
+  <si>
+    <t>Fichier à modifiés : 
+« index.php »
+header.php
+single.php 
+footer.php
+styles.css
+situé sous « /blog/wp-content/themes/twentyseventeen/»</t>
+  </si>
+  <si>
+    <t>« throwback16/blog ».</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1196,6 +1275,41 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF282828"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF282828"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF282828"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1330,7 +1444,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -1339,8 +1453,9 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1453,6 +1568,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1471,9 +1587,23 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Calcul" xfId="2" builtinId="22"/>
     <cellStyle name="Entrée" xfId="7" builtinId="20"/>
     <cellStyle name="Insatisfaisant" xfId="5" builtinId="27"/>
@@ -1481,6 +1611,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="4" builtinId="26"/>
     <cellStyle name="Sortie" xfId="1" builtinId="21"/>
+    <cellStyle name="Texte explicatif" xfId="8" builtinId="53"/>
     <cellStyle name="Vérification" xfId="6" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2068,10 +2199,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="39"/>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="49" t="s">
         <v>206</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -2080,8 +2211,8 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="39"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="48"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="34" t="s">
         <v>203</v>
       </c>
@@ -2090,7 +2221,7 @@
       <c r="B13" s="39">
         <v>10</v>
       </c>
-      <c r="C13" s="51"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="28" t="s">
         <v>205</v>
       </c>
@@ -2272,19 +2403,19 @@
       <c r="B15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="52"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="D16" s="52"/>
+      <c r="D16" s="53"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="21"/>
@@ -2293,10 +2424,10 @@
       <c r="B18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="52"/>
+      <c r="D18" s="53"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="20"/>
@@ -2443,7 +2574,7 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="20"/>
-      <c r="C43" s="53" t="s">
+      <c r="C43" s="54" t="s">
         <v>212</v>
       </c>
       <c r="D43" s="14" t="s">
@@ -2455,7 +2586,7 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="20"/>
-      <c r="C44" s="53"/>
+      <c r="C44" s="54"/>
       <c r="D44" s="14" t="s">
         <v>214</v>
       </c>
@@ -2465,7 +2596,7 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="20"/>
-      <c r="C45" s="53"/>
+      <c r="C45" s="54"/>
       <c r="D45" s="14" t="s">
         <v>215</v>
       </c>
@@ -2612,7 +2743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2862,7 +2993,7 @@
       <c r="B32" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C32" s="48" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2870,7 +3001,7 @@
       <c r="A33" t="s">
         <v>237</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="48" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3352,4 +3483,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.33203125" style="56" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" style="37" customWidth="1"/>
+    <col min="4" max="4" width="60.44140625" style="57" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1"/>
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3"/>
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4"/>
+      <c r="C4"/>
+    </row>
+    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="C8" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="55" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="59"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" s="59"/>
+    </row>
+    <row r="13" spans="2:5" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="B13" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="56" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="56" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>